<commit_message>
add real carbon emission and shareholding ratio
</commit_message>
<xml_diff>
--- a/result1.xlsx
+++ b/result1.xlsx
@@ -446,1105 +446,1099 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>必須為0的投資組合</t>
+          <t>投資組合總和下限</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>投資組合總和下限</t>
+          <t>投資組合總和</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>投資組合總和</t>
+          <t>碳排放量總和</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>碳排放量總和</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>成分股比例</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>成分股比例</t>
+          <t>碳排放量</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>碳排放量</t>
+          <t>原碳排放量總和</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2561009670205502</v>
+        <v>7.679521278575138e-07</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.0173543462775147</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2</v>
+        <v>0.9999999999999866</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8467150730438993</v>
-      </c>
-      <c r="F2" t="n">
-        <v>39.99999999998636</v>
-      </c>
-      <c r="G2" t="inlineStr">
+        <v>6362669.644886436</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>台泥</t>
         </is>
       </c>
+      <c r="G2" t="n">
+        <v>0.007305194805194805</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.02</v>
+        <v>4532790</v>
       </c>
       <c r="I2" t="n">
-        <v>77.39560485559633</v>
+        <v>6362669.644886363</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
+        <v>0.007057694679997888</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>統一</t>
         </is>
       </c>
+      <c r="G3" t="n">
+        <v>0.01176948051948052</v>
+      </c>
       <c r="H3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I3" t="n">
-        <v>43.88784397520523</v>
-      </c>
+        <v>164360</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
+        <v>0.01152240094552985</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>台塑</t>
         </is>
       </c>
+      <c r="G4" t="n">
+        <v>0.01034902597402597</v>
+      </c>
       <c r="H4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I4" t="n">
-        <v>85.85979199113825</v>
-      </c>
+        <v>7943750</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="n">
-        <v>0.01748454501468462</v>
-      </c>
-      <c r="C5" t="n">
-        <v>18</v>
-      </c>
+        <v>0.01733633386977552</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>南亞</t>
         </is>
       </c>
+      <c r="G5" t="n">
+        <v>0.01318993506493507</v>
+      </c>
       <c r="H5" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I5" t="n">
-        <v>69.73680290593639</v>
-      </c>
+        <v>4584340</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="n">
-        <v>0.02437929781624306</v>
+        <v>0.01163484127300442</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>台化</t>
         </is>
       </c>
+      <c r="G6" t="n">
+        <v>0.007508116883116883</v>
+      </c>
       <c r="H6" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I6" t="n">
-        <v>9.417734788764953</v>
-      </c>
+        <v>7865270</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="n">
-        <v>0.01926971741589229</v>
+        <v>0.008638441608324273</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>亞德客-KY</t>
         </is>
       </c>
+      <c r="G7" t="n">
+        <v>0.00578327922077922</v>
+      </c>
       <c r="H7" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I7" t="n">
-        <v>97.5622351636756</v>
-      </c>
+        <v>121410</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="n">
-        <v>0.01905405466929833</v>
+        <v>0.000931225767243647</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>中鋼</t>
         </is>
       </c>
+      <c r="G8" t="n">
+        <v>0.01105925324675325</v>
+      </c>
       <c r="H8" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I8" t="n">
-        <v>76.11397019903529</v>
-      </c>
+        <v>19661420</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="n">
-        <v>0.01937915792618151</v>
+        <v>0.01017987970689211</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>和泰車</t>
         </is>
       </c>
+      <c r="G9" t="n">
+        <v>0.007711038961038961</v>
+      </c>
       <c r="H9" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I9" t="n">
-        <v>78.60643052769538</v>
-      </c>
+        <v>1770</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="n">
-        <v>0.02245056742695855</v>
+        <v>0.007516451259478545</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>光寶科</t>
         </is>
       </c>
+      <c r="G10" t="n">
+        <v>0.00791396103896104</v>
+      </c>
       <c r="H10" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I10" t="n">
-        <v>12.81136326755459</v>
-      </c>
+        <v>185290</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="n">
-        <v>0.02344652166038022</v>
+        <v>0.01581591923339772</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>聯電</t>
         </is>
       </c>
+      <c r="G11" t="n">
+        <v>0.01968344155844156</v>
+      </c>
       <c r="H11" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I11" t="n">
-        <v>45.03859378955671</v>
-      </c>
+        <v>1965690</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="n">
-        <v>0.0241215812900767</v>
+        <v>0.009784626067330177</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>台達電</t>
         </is>
       </c>
+      <c r="G12" t="n">
+        <v>0.02333603896103896</v>
+      </c>
       <c r="H12" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I12" t="n">
-        <v>37.07980242325812</v>
-      </c>
+        <v>187650</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="n">
-        <v>0.01656615390419056</v>
+        <v>0.0148333394858</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>鴻海</t>
         </is>
       </c>
+      <c r="G13" t="n">
+        <v>0.03784496753246753</v>
+      </c>
       <c r="H13" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I13" t="n">
-        <v>92.67649888486018</v>
-      </c>
+        <v>5738140</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="n">
-        <v>0.02086923652536712</v>
+        <v>0.01602840359917868</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>國巨</t>
         </is>
       </c>
+      <c r="G14" t="n">
+        <v>0.008015422077922078</v>
+      </c>
       <c r="H14" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I14" t="n">
-        <v>64.38651200806646</v>
-      </c>
+        <v>117660</v>
+      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="n">
-        <v>0.03029842017618908</v>
+        <v>0.4403355036560276</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>台積電</t>
         </is>
       </c>
+      <c r="G15" t="n">
+        <v>0.4709821428571428</v>
+      </c>
       <c r="H15" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I15" t="n">
-        <v>82.276161327083</v>
-      </c>
+        <v>11558550</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="n">
-        <v>0.02028792388020063</v>
+        <v>0.009403914452477768</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>智邦</t>
         </is>
       </c>
+      <c r="G16" t="n">
+        <v>0.00974025974025974</v>
+      </c>
       <c r="H16" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I16" t="n">
-        <v>44.34141988273311</v>
-      </c>
+        <v>15250</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="n">
-        <v>0.02396697611602204</v>
+        <v>0.011044280069088</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>華碩</t>
         </is>
       </c>
+      <c r="G17" t="n">
+        <v>0.009334415584415584</v>
+      </c>
       <c r="H17" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I17" t="n">
-        <v>22.72387217847769</v>
-      </c>
+        <v>18730</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="n">
-        <v>0.01937938136978728</v>
+        <v>0.008832045490875216</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>瑞昱</t>
         </is>
       </c>
+      <c r="G18" t="n">
+        <v>0.007508116883116883</v>
+      </c>
       <c r="H18" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I18" t="n">
-        <v>55.45847870158348</v>
-      </c>
+        <v>26460</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="n">
-        <v>0.02807110501989341</v>
+        <v>0.01109152056186666</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>廣達</t>
         </is>
       </c>
+      <c r="G19" t="n">
+        <v>0.01826298701298701</v>
+      </c>
       <c r="H19" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I19" t="n">
-        <v>6.381725610417533</v>
-      </c>
+        <v>317270</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.009656675765323235</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>研華</t>
         </is>
       </c>
+      <c r="G20" t="n">
+        <v>0.005478896103896104</v>
+      </c>
       <c r="H20" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I20" t="n">
-        <v>82.7631171992582</v>
-      </c>
+        <v>33380</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="n">
-        <v>0.02119937346057751</v>
+        <v>0.01340501290181296</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>南亞科</t>
         </is>
       </c>
+      <c r="G21" t="n">
+        <v>0.002029220779220779</v>
+      </c>
       <c r="H21" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I21" t="n">
-        <v>63.16643991220649</v>
-      </c>
+        <v>440950</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="n">
-        <v>2.46269631857499e-10</v>
+        <v>0.0127047388858888</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>中華電</t>
         </is>
       </c>
+      <c r="G22" t="n">
+        <v>0.01552353896103896</v>
+      </c>
       <c r="H22" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I22" t="n">
-        <v>75.80877400853738</v>
-      </c>
+        <v>714100</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="n">
-        <v>0.02288240928313353</v>
+        <v>0.01130603282691885</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>聯發科</t>
         </is>
       </c>
+      <c r="G23" t="n">
+        <v>0.04809253246753247</v>
+      </c>
       <c r="H23" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I23" t="n">
-        <v>35.45259681298683</v>
-      </c>
+        <v>90320</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="n">
-        <v>0.02011772902533263</v>
+        <v>0.01736913695245337</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>長榮</t>
         </is>
       </c>
+      <c r="G24" t="n">
+        <v>0.003855519480519481</v>
+      </c>
       <c r="H24" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I24" t="n">
-        <v>97.06980243949033</v>
-      </c>
+        <v>8185210</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="n">
-        <v>0.008920950820166971</v>
+        <v>0.008818865122257822</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>彰銀</t>
         </is>
       </c>
+      <c r="G25" t="n">
+        <v>0.004159902597402597</v>
+      </c>
       <c r="H25" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I25" t="n">
-        <v>89.31211213221977</v>
-      </c>
+        <v>17090</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="n">
-        <v>0.008857085835813377</v>
+        <v>0.008838188700446548</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>華南金</t>
         </is>
       </c>
+      <c r="G26" t="n">
+        <v>0.007609577922077922</v>
+      </c>
       <c r="H26" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I26" t="n">
-        <v>77.83834970737618</v>
-      </c>
+        <v>20180</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="n">
-        <v>0.02401137908382196</v>
+        <v>0.007958493681170969</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>富邦金</t>
         </is>
       </c>
+      <c r="G27" t="n">
+        <v>0.01684253246753247</v>
+      </c>
       <c r="H27" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I27" t="n">
-        <v>19.46387078519676</v>
-      </c>
+        <v>57840</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="n">
-        <v>0.02020465335807109</v>
+        <v>0.007825662257661173</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>國泰金</t>
         </is>
       </c>
+      <c r="G28" t="n">
+        <v>0.01440746753246753</v>
+      </c>
       <c r="H28" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I28" t="n">
-        <v>46.67210037270342</v>
-      </c>
+        <v>59750</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="n">
-        <v>0.02496605803807772</v>
+        <v>0.00942162968423188</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>開發金</t>
         </is>
       </c>
+      <c r="G29" t="n">
+        <v>0.006797889610389611</v>
+      </c>
       <c r="H29" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I29" t="n">
-        <v>4.380376578722878</v>
-      </c>
+        <v>21500</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="n">
-        <v>0.02392137589114833</v>
+        <v>0.008999285263483925</v>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>玉山金</t>
         </is>
       </c>
+      <c r="G30" t="n">
+        <v>0.01298701298701299</v>
+      </c>
       <c r="H30" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I30" t="n">
-        <v>15.42894920675478</v>
-      </c>
+        <v>22140</v>
+      </c>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="n">
-        <v>0.01782632620352453</v>
+        <v>0.00929168105004383</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>元大金</t>
         </is>
       </c>
+      <c r="G31" t="n">
+        <v>0.01075487012987013</v>
+      </c>
       <c r="H31" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I31" t="n">
-        <v>68.30489532424546</v>
-      </c>
+        <v>20000</v>
+      </c>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="n">
-        <v>0.01277484588455894</v>
+        <v>0.008888226581556359</v>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>兆豐金</t>
         </is>
       </c>
+      <c r="G32" t="n">
+        <v>0.01501623376623377</v>
+      </c>
       <c r="H32" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I32" t="n">
-        <v>74.47621559078172</v>
-      </c>
+        <v>20180</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="n">
-        <v>0.01091791940246494</v>
+        <v>0.008994947258714629</v>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>台新金</t>
         </is>
       </c>
+      <c r="G33" t="n">
+        <v>0.007305194805194805</v>
+      </c>
       <c r="H33" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I33" t="n">
-        <v>96.750973243421</v>
-      </c>
+        <v>21450</v>
+      </c>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="n">
-        <v>0.02098130793497438</v>
+        <v>0.008917501380964286</v>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>永豐金</t>
         </is>
       </c>
+      <c r="G34" t="n">
+        <v>0.007406655844155844</v>
+      </c>
       <c r="H34" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I34" t="n">
-        <v>32.58253581381519</v>
-      </c>
+        <v>19210</v>
+      </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="n">
-        <v>0.02225824090831181</v>
+        <v>0.00793617779919404</v>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>中信金</t>
         </is>
       </c>
+      <c r="G35" t="n">
+        <v>0.01674107142857143</v>
+      </c>
       <c r="H35" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I35" t="n">
-        <v>37.04597060348689</v>
-      </c>
+        <v>43730</v>
+      </c>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="n">
-        <v>0.0165865516520427</v>
+        <v>0.008807052206670551</v>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>第一金</t>
         </is>
       </c>
+      <c r="G36" t="n">
+        <v>0.01004464285714286</v>
+      </c>
       <c r="H36" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I36" t="n">
-        <v>46.95558112758079</v>
-      </c>
+        <v>21520</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="n">
-        <v>0.01714574718294548</v>
+        <v>0.0154632480770698</v>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>統一超</t>
         </is>
       </c>
+      <c r="G37" t="n">
+        <v>0.005174512987012987</v>
+      </c>
       <c r="H37" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I37" t="n">
-        <v>18.94713590842857</v>
-      </c>
+        <v>534480</v>
+      </c>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="n">
-        <v>0.02213075354193033</v>
+        <v>0.0102859526372673</v>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>大立光</t>
         </is>
       </c>
+      <c r="G38" t="n">
+        <v>0.008319805194805194</v>
+      </c>
       <c r="H38" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I38" t="n">
-        <v>12.99215053354716</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="n">
-        <v>0.022973239994033</v>
+        <v>0.01469286792745656</v>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>聯詠</t>
         </is>
       </c>
+      <c r="G39" t="n">
+        <v>0.01004464285714286</v>
+      </c>
       <c r="H39" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I39" t="n">
-        <v>47.57049262259338</v>
-      </c>
+        <v>18570</v>
+      </c>
+      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="n">
-        <v>0.02224444439508198</v>
+        <v>0.05250042295191245</v>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>欣興</t>
         </is>
       </c>
+      <c r="G40" t="n">
+        <v>0.007711038961038961</v>
+      </c>
       <c r="H40" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I40" t="n">
-        <v>22.69093490508841</v>
-      </c>
+        <v>942080</v>
+      </c>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="n">
-        <v>6.606976567042785e-09</v>
+        <v>0.008969415380656416</v>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>台灣大</t>
         </is>
       </c>
+      <c r="G41" t="n">
+        <v>0.00578327922077922</v>
+      </c>
       <c r="H41" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I41" t="n">
-        <v>66.98139946825104</v>
-      </c>
+        <v>287470</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="n">
-        <v>0.02034583451644985</v>
+        <v>0.01074446416936457</v>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>緯創</t>
         </is>
       </c>
+      <c r="G42" t="n">
+        <v>0.009131493506493506</v>
+      </c>
       <c r="H42" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I42" t="n">
-        <v>43.71519188723308</v>
-      </c>
+        <v>323180</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="n">
-        <v>0.01728509912721255</v>
+        <v>0.009942100260192434</v>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>日月光投控</t>
         </is>
       </c>
+      <c r="G43" t="n">
+        <v>0.01481331168831169</v>
+      </c>
       <c r="H43" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I43" t="n">
-        <v>83.26781960578374</v>
-      </c>
+        <v>1762240</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="n">
-        <v>0.002328189276650159</v>
+        <v>0.008674469250405877</v>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>遠傳</t>
         </is>
       </c>
+      <c r="G44" t="n">
+        <v>0.004464285714285714</v>
+      </c>
       <c r="H44" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I44" t="n">
-        <v>70.02651020022491</v>
-      </c>
+        <v>291490</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="n">
-        <v>0.01688053051465933</v>
+        <v>0.008903427931494675</v>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>和碩</t>
         </is>
       </c>
+      <c r="G45" t="n">
+        <v>0.005681818181818182</v>
+      </c>
       <c r="H45" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I45" t="n">
-        <v>31.23666413820411</v>
-      </c>
+        <v>441600</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="n">
-        <v>0.01741140345207217</v>
+        <v>0.008090830019185874</v>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>中租-KY</t>
         </is>
       </c>
+      <c r="G46" t="n">
+        <v>0.00882711038961039</v>
+      </c>
       <c r="H46" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I46" t="n">
-        <v>83.2259801395201</v>
-      </c>
+        <v>3390</v>
+      </c>
+      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="n">
-        <v>0.0147162687363708</v>
+        <v>0.008418134790429592</v>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>上海商銀</t>
         </is>
       </c>
+      <c r="G47" t="n">
+        <v>0.00578327922077922</v>
+      </c>
       <c r="H47" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I47" t="n">
-        <v>80.47643574968019</v>
-      </c>
+        <v>8189.999999999999</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="n">
-        <v>0.0126843384679217</v>
+        <v>0.007977274801798887</v>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>合庫金</t>
         </is>
       </c>
+      <c r="G48" t="n">
+        <v>0.0096387987012987</v>
+      </c>
       <c r="H48" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I48" t="n">
-        <v>38.74783790301745</v>
-      </c>
+        <v>26060</v>
+      </c>
+      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="n">
-        <v>0.01738943202278571</v>
+        <v>0.02187611337838303</v>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>台塑化</t>
         </is>
       </c>
+      <c r="G49" t="n">
+        <v>0.00395698051948052</v>
+      </c>
       <c r="H49" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I49" t="n">
-        <v>28.83281039302441</v>
-      </c>
+        <v>24424100</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="n">
-        <v>0.01872741153757482</v>
+        <v>0.008310241294267731</v>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>緯穎</t>
         </is>
       </c>
+      <c r="G50" t="n">
+        <v>0.005275974025974026</v>
+      </c>
       <c r="H50" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I50" t="n">
-        <v>68.24955039749754</v>
-      </c>
+        <v>20360</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="n">
-        <v>0.01900152643157929</v>
+        <v>0.006670560807505233</v>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>豐泰</t>
         </is>
       </c>
+      <c r="G51" t="n">
+        <v>0.003043831168831169</v>
+      </c>
       <c r="H51" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I51" t="n">
-        <v>13.97524836093098</v>
-      </c>
+        <v>249040</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>